<commit_message>
Chore Novos Dados Extraídos
</commit_message>
<xml_diff>
--- a/dados_raspados_PA.xlsx
+++ b/dados_raspados_PA.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G418"/>
+  <dimension ref="A1:G431"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17388,29 +17388,29 @@
     <row r="415">
       <c r="A415" t="inlineStr">
         <is>
-          <t>E M E I E F BOM JARDIM I</t>
+          <t>E M E F MARIA DE LOURDES CASADINI DA SILVA</t>
         </is>
       </c>
       <c r="B415" t="inlineStr">
         <is>
-          <t>RODOVIA TRANSAMAZONICA, KM 45 COBRA CHOCA. ZONA RURAL. 68383-000 Vitória do Xingu - PA.</t>
+          <t>RUA ANTONIO ALVES DE CARVALHO, 56 ESCOLA CASADINI. EXPANSAO. 68560-000 Santana do Araguaia - PA.</t>
         </is>
       </c>
       <c r="C415" t="inlineStr">
         <is>
-          <t>(93) 99212-7520</t>
+          <t>94.</t>
         </is>
       </c>
       <c r="D415" t="inlineStr">
         <is>
           <t xml:space="preserve">
-15111040</t>
+15524655</t>
         </is>
       </c>
       <c r="E415" t="inlineStr">
         <is>
           <t xml:space="preserve">
-Rural</t>
+Urbana</t>
         </is>
       </c>
       <c r="F415" t="inlineStr">
@@ -17422,30 +17422,30 @@
       <c r="G415" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        Ensino Infantil, Ensino Fundamental</t>
+                        Ensino Infantil, Ensino Fundamental, Anos Iniciais, Anos Finais</t>
         </is>
       </c>
     </row>
     <row r="416">
       <c r="A416" t="inlineStr">
         <is>
-          <t>E M E I E F AVELINA MARIA DA SILVA</t>
+          <t>E M E F VILA NOVA</t>
         </is>
       </c>
       <c r="B416" t="inlineStr">
         <is>
-          <t>RODOVIA ERNESTO ACIOLY, KM 40 RAMAL DO COCO. ZONA RURAL. 68383-000 Vitória do Xingu - PA.</t>
+          <t>VILA NOVA MARO - RIO ARAPIUNS, 68115-000 Santarém - PA.</t>
         </is>
       </c>
       <c r="C416" t="inlineStr">
         <is>
-          <t>(93) 99212-7520</t>
+          <t>Informação indisponível</t>
         </is>
       </c>
       <c r="D416" t="inlineStr">
         <is>
           <t xml:space="preserve">
-15105920</t>
+15156770</t>
         </is>
       </c>
       <c r="E416" t="inlineStr">
@@ -17470,64 +17470,64 @@
     <row r="417">
       <c r="A417" t="inlineStr">
         <is>
-          <t>E M E I E F PADRE EURICO KRAUTLER</t>
+          <t>EEEM ALVARO ADOLFO DA SILVEIRA</t>
         </is>
       </c>
       <c r="B417" t="inlineStr">
         <is>
-          <t>RODOVIA ERNESTO ACIOLY KM 20, SN ZONA RURAL. 68383-000 Vitória do Xingu - PA.</t>
+          <t>AV MARECHAL RONDON, SN SANTA CLARA. 68005-120 Santarém - PA.</t>
         </is>
       </c>
       <c r="C417" t="inlineStr">
         <is>
-          <t>93.</t>
+          <t>(93) 3522-2329</t>
         </is>
       </c>
       <c r="D417" t="inlineStr">
         <is>
           <t xml:space="preserve">
-15111270</t>
+15011372</t>
         </is>
       </c>
       <c r="E417" t="inlineStr">
         <is>
           <t xml:space="preserve">
-Rural</t>
+Urbana</t>
         </is>
       </c>
       <c r="F417" t="inlineStr">
         <is>
           <t xml:space="preserve">
-Municipal</t>
+Estadual</t>
         </is>
       </c>
       <c r="G417" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        Ensino Infantil, Ensino Fundamental</t>
+                        Ensino Médio</t>
         </is>
       </c>
     </row>
     <row r="418">
       <c r="A418" t="inlineStr">
         <is>
-          <t>E M E I F PADRE JOAO LUIZ PURGUY</t>
+          <t>E M E F NSRA DAS GRACAS</t>
         </is>
       </c>
       <c r="B418" t="inlineStr">
         <is>
-          <t>AV JADER FONTENELLE BARBALHO, SN DISTRITO RIO VERMELHO. 68559-500 Xinguara - PA.</t>
+          <t>COMUNIDADE DE AMARI, ARAPIUNS. 68115-000 Santarém - PA.</t>
         </is>
       </c>
       <c r="C418" t="inlineStr">
         <is>
-          <t>(94) 99257-8784</t>
+          <t>..</t>
         </is>
       </c>
       <c r="D418" t="inlineStr">
         <is>
           <t xml:space="preserve">
-15134296</t>
+15013260</t>
         </is>
       </c>
       <c r="E418" t="inlineStr">
@@ -17543,6 +17543,539 @@
         </is>
       </c>
       <c r="G418" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        Ensino Fundamental</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>E M E F SANTISSIMA TRINDADE</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>SANTISSIMA TRINDADE- VILA DO ARITAPERA, VARZEA. 68124-000 Santarém - PA.</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>..</t>
+        </is>
+      </c>
+      <c r="D419" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+15140849</t>
+        </is>
+      </c>
+      <c r="E419" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Rural</t>
+        </is>
+      </c>
+      <c r="F419" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Municipal</t>
+        </is>
+      </c>
+      <c r="G419" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        Ensino Infantil, Ensino Fundamental</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>E M E I E F PROF OLINDO LUIZ DO CARMO NEVES</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>RUA ITUQUI, S/N IGREJA DO AMPARO. AMPARO. 68035-670 Santarém - PA.</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>(93) 99121-8227</t>
+        </is>
+      </c>
+      <c r="D420" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+15013626</t>
+        </is>
+      </c>
+      <c r="E420" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Urbana</t>
+        </is>
+      </c>
+      <c r="F420" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Municipal</t>
+        </is>
+      </c>
+      <c r="G420" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        Ensino Infantil, Ensino Fundamental</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>E M E F VINTE DE JULHO</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>COMUNIDADE CORREIO DO TAPARA, VARZEA. 68124-000 Santarém - PA.</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>Informação indisponível</t>
+        </is>
+      </c>
+      <c r="D421" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+15147991</t>
+        </is>
+      </c>
+      <c r="E421" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Rural</t>
+        </is>
+      </c>
+      <c r="F421" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Municipal</t>
+        </is>
+      </c>
+      <c r="G421" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        Ensino Infantil, Ensino Fundamental</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>E M E F CEL MARIO FERNANDES IMBIRIBA</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>RUA CASTELO BRANCO, INTERVENTORIA. 68015-260 Santarém - PA.</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>(93) 3523-4313</t>
+        </is>
+      </c>
+      <c r="D422" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+15012115</t>
+        </is>
+      </c>
+      <c r="E422" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Urbana</t>
+        </is>
+      </c>
+      <c r="F422" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Municipal</t>
+        </is>
+      </c>
+      <c r="G422" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        Ensino Infantil, Ensino Fundamental</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>E M E I E F NOVA ESPERANCA</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>COMUNIDADE NOVA ESPERANCA DO ITUQUI, S/N ZONA RURAL. PLANALTO. 68128-000 Santarém - PA.</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>Informação indisponível</t>
+        </is>
+      </c>
+      <c r="D423" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+15540650</t>
+        </is>
+      </c>
+      <c r="E423" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Rural</t>
+        </is>
+      </c>
+      <c r="F423" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Municipal</t>
+        </is>
+      </c>
+      <c r="G423" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        Ensino Infantil, Ensino Fundamental</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>E M E F JOSE DE MELO FILHO</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>VILA DE AMORIM, RIO TAPAJOS. ZONA RURAL. 68115-000 Santarém - PA.</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>(93) 3584-4125</t>
+        </is>
+      </c>
+      <c r="D424" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+15015955</t>
+        </is>
+      </c>
+      <c r="E424" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Rural</t>
+        </is>
+      </c>
+      <c r="F424" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Municipal</t>
+        </is>
+      </c>
+      <c r="G424" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        Ensino Infantil, Ensino Fundamental</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>E M E F RAIMUNDA DE LIRA MAIA</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>TRAVESSA B, S/N ELCIONE BARBALHO. 68040-050 Santarém - PA.</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>(93) 99182-2030</t>
+        </is>
+      </c>
+      <c r="D425" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+15567044</t>
+        </is>
+      </c>
+      <c r="E425" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Urbana</t>
+        </is>
+      </c>
+      <c r="F425" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Municipal</t>
+        </is>
+      </c>
+      <c r="G425" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        Ensino Infantil, Ensino Fundamental</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>EEEF RICHARD HENNINGTON</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>TRAVESSA XINGU, 997 ENTRE AVENIDA PALHAO. DIAMANTINO. 68020-140 Santarém - PA.</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>(93) 3524-3435</t>
+        </is>
+      </c>
+      <c r="D426" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+15011712</t>
+        </is>
+      </c>
+      <c r="E426" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Urbana</t>
+        </is>
+      </c>
+      <c r="F426" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Estadual</t>
+        </is>
+      </c>
+      <c r="G426" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        Ensino Fundamental</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>E M E F SAO TOME</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>COMUNIDADE SAO PEDRO, PLANALTO. 68123-000 Santarém - PA.</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>(93) 3596-2063</t>
+        </is>
+      </c>
+      <c r="D427" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+15589404</t>
+        </is>
+      </c>
+      <c r="E427" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Rural</t>
+        </is>
+      </c>
+      <c r="F427" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Municipal</t>
+        </is>
+      </c>
+      <c r="G427" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        Ensino Infantil, Ensino Fundamental</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>E M E F NOSSA SRA DE FATIMA</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>ALDEIA NOVA VISTA- ARAPIUNS, ARAPIUNS. 68115-000 Santarém - PA.</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>Informação indisponível</t>
+        </is>
+      </c>
+      <c r="D428" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+15013049</t>
+        </is>
+      </c>
+      <c r="E428" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Rural</t>
+        </is>
+      </c>
+      <c r="F428" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Municipal</t>
+        </is>
+      </c>
+      <c r="G428" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        Ensino Infantil, Ensino Fundamental, Anos Finais</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>E M E F JAYME BARCESSAT</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>HIDRELETRICA DE CURUA-UNA, PA 370 KM74, PLANALTO. 68010-000 Santarém - PA.</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>93.</t>
+        </is>
+      </c>
+      <c r="D429" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+15011232</t>
+        </is>
+      </c>
+      <c r="E429" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Rural</t>
+        </is>
+      </c>
+      <c r="F429" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Municipal</t>
+        </is>
+      </c>
+      <c r="G429" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        Ensino Infantil, Ensino Fundamental</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>EEEM JULIA PASSARINHO - ANEXO I</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>AVENIDA COSTA E SILVA, SN PROX. POSTO DE SAUD. MARARU. 68050-070 Santarém - PA.</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>(93) 3523-5994</t>
+        </is>
+      </c>
+      <c r="D430" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+15170080</t>
+        </is>
+      </c>
+      <c r="E430" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Urbana</t>
+        </is>
+      </c>
+      <c r="F430" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Estadual</t>
+        </is>
+      </c>
+      <c r="G430" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        Ensino Médio</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>E M E F STA TEREZINHA</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>BOCA DE CIMA DO ARITAPERA, VARZEA. 68124-000 Santarém - PA.</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>(93) 99163-8872</t>
+        </is>
+      </c>
+      <c r="D431" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+15015084</t>
+        </is>
+      </c>
+      <c r="E431" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Rural</t>
+        </is>
+      </c>
+      <c r="F431" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Municipal</t>
+        </is>
+      </c>
+      <c r="G431" t="inlineStr">
         <is>
           <t xml:space="preserve">
                         Ensino Infantil, Ensino Fundamental</t>

</xml_diff>